<commit_message>
New Card DTO using card name, imageId and total number of that specific card in collection
</commit_message>
<xml_diff>
--- a/cards.json.xlsx
+++ b/cards.json.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\PC2\Facultate\Licenta\DuelMasters\IntelliJ\DuelMastersServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD66CD1-FCF2-42A4-B884-509CC97C570F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE99FEB2-1041-442C-BD1A-4178CD45B3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1080" windowWidth="23310" windowHeight="12390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10628" uniqueCount="3681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10629" uniqueCount="3683">
   <si>
     <t>cards</t>
   </si>
@@ -11248,9 +11248,6 @@
     <t>Choose0(1, BZ0) + SEL:Give(SL0, EOT)</t>
   </si>
   <si>
-    <t>Choose0(1, BZ0) + SEL:Give(TCG5000, EOT)</t>
-  </si>
-  <si>
     <t>Choose0(1, BZ0) + SEL:Give(DB0, EOT)</t>
   </si>
   <si>
@@ -11774,6 +11771,15 @@
   </si>
   <si>
     <t>82 DONE</t>
+  </si>
+  <si>
+    <t>OP{Choose0(2, MN0) + SEL:MTH}</t>
+  </si>
+  <si>
+    <t>Choose0(1, BZ0) + SEL:Give(TCCG5000, EOT)</t>
+  </si>
+  <si>
+    <t>38 DONE</t>
   </si>
 </sst>
 </file>
@@ -48040,8 +48046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F3F974-4C98-45F8-96F5-103C5419490D}">
   <dimension ref="A3:H376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E359" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G375" sqref="G375"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48653,7 +48659,7 @@
         <v>2103</v>
       </c>
       <c r="G76" s="33" t="s">
-        <v>3485</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -48744,7 +48750,7 @@
         <v>2115</v>
       </c>
       <c r="G81" s="33" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -48961,7 +48967,7 @@
         <v>3497</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
       <c r="E97" s="4" t="s">
@@ -48974,7 +48980,7 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
       <c r="E98" s="4" t="s">
@@ -48985,7 +48991,7 @@
       </c>
       <c r="G98" s="34"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="E99" s="4" t="s">
@@ -48996,7 +49002,7 @@
       </c>
       <c r="G99" s="34"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="E100" s="4" t="s">
@@ -49009,7 +49015,7 @@
         <v>3498</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="E101" s="4" t="s">
@@ -49022,7 +49028,7 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="E102" s="4" t="s">
@@ -49033,7 +49039,7 @@
       </c>
       <c r="G102" s="33"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="E103" s="4" t="s">
@@ -49046,7 +49052,7 @@
         <v>3491</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="E104" s="4" t="s">
@@ -49059,7 +49065,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
       <c r="E105" s="4" t="s">
@@ -49072,7 +49078,7 @@
         <v>3501</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
       <c r="E106" s="4" t="s">
@@ -49084,8 +49090,11 @@
       <c r="G106" s="33" t="s">
         <v>3502</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>3556</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
       <c r="E107" s="4" t="s">
@@ -49098,7 +49107,7 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
       <c r="E108" s="4" t="s">
@@ -49111,7 +49120,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="E109" s="4" t="s">
@@ -49121,10 +49130,10 @@
         <v>2138</v>
       </c>
       <c r="G109" s="33" t="s">
-        <v>3505</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
       <c r="E110" s="4" t="s">
@@ -49134,10 +49143,10 @@
         <v>2139</v>
       </c>
       <c r="G110" s="33" t="s">
-        <v>3506</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
       <c r="E111" s="4" t="s">
@@ -49147,10 +49156,10 @@
         <v>2140</v>
       </c>
       <c r="G111" s="33" t="s">
-        <v>3507</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3506</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="E112" s="4" t="s">
@@ -49242,7 +49251,7 @@
         <v>2147</v>
       </c>
       <c r="G118" s="33" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.25">
@@ -49253,7 +49262,7 @@
         <v>2148</v>
       </c>
       <c r="G119" s="33" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
@@ -49287,10 +49296,10 @@
         <v>2150</v>
       </c>
       <c r="G121" s="33" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="H121" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.25">
@@ -49307,7 +49316,7 @@
         <v>2151</v>
       </c>
       <c r="G122" s="33" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.25">
@@ -49324,7 +49333,7 @@
         <v>2152</v>
       </c>
       <c r="G123" s="33" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
@@ -49358,7 +49367,7 @@
         <v>2153</v>
       </c>
       <c r="G125" s="33" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
@@ -49375,7 +49384,7 @@
         <v>2204</v>
       </c>
       <c r="G126" s="33" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.25">
@@ -49386,7 +49395,7 @@
         <v>1905</v>
       </c>
       <c r="H127" t="s">
-        <v>3678</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
@@ -49419,7 +49428,7 @@
         <v>1303</v>
       </c>
       <c r="G132" s="33" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
@@ -49430,7 +49439,7 @@
         <v>1306</v>
       </c>
       <c r="G133" s="33" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
@@ -49447,7 +49456,7 @@
         <v>1311</v>
       </c>
       <c r="G134" s="33" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
@@ -49498,7 +49507,7 @@
         <v>1327</v>
       </c>
       <c r="G137" s="33" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
@@ -49532,7 +49541,7 @@
         <v>2330</v>
       </c>
       <c r="G139" s="33" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
@@ -49549,7 +49558,7 @@
         <v>2331</v>
       </c>
       <c r="G140" s="33" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
@@ -49590,7 +49599,7 @@
         <v>2337</v>
       </c>
       <c r="G143" s="33" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
@@ -49601,7 +49610,7 @@
         <v>2338</v>
       </c>
       <c r="G144" s="47" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
@@ -49618,7 +49627,7 @@
         <v>2340</v>
       </c>
       <c r="G145" s="33" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
@@ -49635,7 +49644,7 @@
         <v>2342</v>
       </c>
       <c r="G146" s="33" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
@@ -49669,7 +49678,7 @@
         <v>2346</v>
       </c>
       <c r="G148" s="33" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
@@ -49703,7 +49712,7 @@
         <v>2349</v>
       </c>
       <c r="G150" s="33" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
@@ -49714,7 +49723,7 @@
         <v>2350</v>
       </c>
       <c r="G151" s="33" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
@@ -49742,7 +49751,7 @@
         <v>2353</v>
       </c>
       <c r="G153" s="33" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
@@ -49753,7 +49762,7 @@
         <v>2355</v>
       </c>
       <c r="G154" s="33" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
@@ -49764,7 +49773,7 @@
         <v>2356</v>
       </c>
       <c r="G155" s="33" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
@@ -49775,7 +49784,7 @@
         <v>2357</v>
       </c>
       <c r="G156" s="33" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
@@ -49786,7 +49795,7 @@
         <v>1507</v>
       </c>
       <c r="G157" s="33" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
@@ -49797,7 +49806,7 @@
         <v>1485</v>
       </c>
       <c r="G158" s="33" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
@@ -49819,7 +49828,7 @@
         <v>1551</v>
       </c>
       <c r="G160" s="33" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.25">
@@ -49830,10 +49839,10 @@
         <v>2363</v>
       </c>
       <c r="G161" s="33" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="H161" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="162" spans="2:8" x14ac:dyDescent="0.25">
@@ -49844,7 +49853,7 @@
         <v>2365</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="163" spans="2:8" x14ac:dyDescent="0.25">
@@ -49855,7 +49864,7 @@
         <v>1472</v>
       </c>
       <c r="G163" s="33" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="164" spans="2:8" x14ac:dyDescent="0.25">
@@ -49866,7 +49875,7 @@
         <v>1522</v>
       </c>
       <c r="G164" s="33" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="165" spans="2:8" x14ac:dyDescent="0.25">
@@ -49877,10 +49886,10 @@
         <v>1443</v>
       </c>
       <c r="G165" s="33" t="s">
+        <v>3540</v>
+      </c>
+      <c r="H165" t="s">
         <v>3541</v>
-      </c>
-      <c r="H165" t="s">
-        <v>3542</v>
       </c>
     </row>
     <row r="166" spans="2:8" x14ac:dyDescent="0.25">
@@ -49891,10 +49900,10 @@
         <v>1436</v>
       </c>
       <c r="G166" s="33" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="H166" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="167" spans="2:8" x14ac:dyDescent="0.25">
@@ -49905,7 +49914,7 @@
         <v>1539</v>
       </c>
       <c r="G167" s="33" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="168" spans="2:8" x14ac:dyDescent="0.25">
@@ -49922,7 +49931,7 @@
         <v>1435</v>
       </c>
       <c r="G168" s="33" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="169" spans="2:8" x14ac:dyDescent="0.25">
@@ -49939,7 +49948,7 @@
         <v>1400</v>
       </c>
       <c r="G169" s="33" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="170" spans="2:8" x14ac:dyDescent="0.25">
@@ -49956,7 +49965,7 @@
         <v>1548</v>
       </c>
       <c r="G170" s="33" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="171" spans="2:8" x14ac:dyDescent="0.25">
@@ -49973,7 +49982,7 @@
         <v>2375</v>
       </c>
       <c r="G171" s="33" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="172" spans="2:8" x14ac:dyDescent="0.25">
@@ -50007,7 +50016,7 @@
         <v>1563</v>
       </c>
       <c r="G173" s="33" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
     </row>
     <row r="174" spans="2:8" x14ac:dyDescent="0.25">
@@ -50024,7 +50033,7 @@
         <v>1493</v>
       </c>
       <c r="G174" s="33" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="175" spans="2:8" x14ac:dyDescent="0.25">
@@ -50041,7 +50050,7 @@
         <v>1366</v>
       </c>
       <c r="G175" s="33" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="176" spans="2:8" x14ac:dyDescent="0.25">
@@ -50058,7 +50067,7 @@
         <v>1444</v>
       </c>
       <c r="G176" s="33" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.25">
@@ -50075,7 +50084,7 @@
         <v>1389</v>
       </c>
       <c r="G177" s="33" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.25">
@@ -50092,7 +50101,7 @@
         <v>1502</v>
       </c>
       <c r="G178" s="33" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="179" spans="2:8" x14ac:dyDescent="0.25">
@@ -50109,7 +50118,7 @@
         <v>1534</v>
       </c>
       <c r="G179" s="33" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
@@ -50126,7 +50135,7 @@
         <v>1397</v>
       </c>
       <c r="G180" s="33" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="181" spans="2:8" x14ac:dyDescent="0.25">
@@ -50143,7 +50152,7 @@
         <v>1508</v>
       </c>
       <c r="G181" s="33" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
     </row>
     <row r="182" spans="2:8" x14ac:dyDescent="0.25">
@@ -50160,7 +50169,7 @@
         <v>1369</v>
       </c>
       <c r="G182" s="33" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.25">
@@ -50180,7 +50189,7 @@
         <v>3461</v>
       </c>
       <c r="H183" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="184" spans="2:8" x14ac:dyDescent="0.25">
@@ -50200,7 +50209,7 @@
         <v>3462</v>
       </c>
       <c r="H184" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="185" spans="2:8" x14ac:dyDescent="0.25">
@@ -50211,7 +50220,7 @@
         <v>2903</v>
       </c>
       <c r="H185" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="186" spans="2:8" x14ac:dyDescent="0.25">
@@ -50247,7 +50256,7 @@
         <v>2403</v>
       </c>
       <c r="G188" s="33" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
@@ -50264,7 +50273,7 @@
         <v>2414</v>
       </c>
       <c r="G189" s="33" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
     </row>
     <row r="190" spans="2:8" x14ac:dyDescent="0.25">
@@ -50275,7 +50284,7 @@
         <v>2444</v>
       </c>
       <c r="G190" s="33" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.25">
@@ -50292,7 +50301,7 @@
         <v>2446</v>
       </c>
       <c r="G191" s="33" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="192" spans="2:8" x14ac:dyDescent="0.25">
@@ -50309,7 +50318,7 @@
         <v>2449</v>
       </c>
       <c r="G192" s="33" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
     </row>
     <row r="193" spans="2:8" x14ac:dyDescent="0.25">
@@ -50341,7 +50350,7 @@
         <v>2452</v>
       </c>
       <c r="G194" s="33" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
     </row>
     <row r="195" spans="2:8" x14ac:dyDescent="0.25">
@@ -50358,7 +50367,7 @@
         <v>2407</v>
       </c>
       <c r="G195" s="33" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
     </row>
     <row r="196" spans="2:8" x14ac:dyDescent="0.25">
@@ -50375,7 +50384,7 @@
         <v>2404</v>
       </c>
       <c r="G196" s="33" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
     </row>
     <row r="197" spans="2:8" x14ac:dyDescent="0.25">
@@ -50392,7 +50401,7 @@
         <v>2458</v>
       </c>
       <c r="G197" s="33" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
     </row>
     <row r="198" spans="2:8" x14ac:dyDescent="0.25">
@@ -50403,7 +50412,7 @@
         <v>2459</v>
       </c>
       <c r="G198" s="33" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="199" spans="2:8" x14ac:dyDescent="0.25">
@@ -50414,7 +50423,7 @@
         <v>2461</v>
       </c>
       <c r="G199" s="33" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="200" spans="2:8" x14ac:dyDescent="0.25">
@@ -50431,7 +50440,7 @@
         <v>3473</v>
       </c>
       <c r="G200" s="33" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="201" spans="2:8" x14ac:dyDescent="0.25">
@@ -50448,7 +50457,7 @@
         <v>2464</v>
       </c>
       <c r="G201" s="33" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="202" spans="2:8" x14ac:dyDescent="0.25">
@@ -50465,10 +50474,10 @@
         <v>2406</v>
       </c>
       <c r="G202" s="33" t="s">
+        <v>3570</v>
+      </c>
+      <c r="H202" t="s">
         <v>3571</v>
-      </c>
-      <c r="H202" t="s">
-        <v>3572</v>
       </c>
     </row>
     <row r="203" spans="2:8" x14ac:dyDescent="0.25">
@@ -50485,7 +50494,7 @@
         <v>1541</v>
       </c>
       <c r="G203" s="33" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
     </row>
     <row r="204" spans="2:8" x14ac:dyDescent="0.25">
@@ -50502,7 +50511,7 @@
         <v>1335</v>
       </c>
       <c r="G204" s="33" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="205" spans="2:8" x14ac:dyDescent="0.25">
@@ -50516,7 +50525,7 @@
         <v>1536</v>
       </c>
       <c r="G205" s="33" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
     </row>
     <row r="206" spans="2:8" x14ac:dyDescent="0.25">
@@ -50530,7 +50539,7 @@
         <v>1329</v>
       </c>
       <c r="G206" s="33" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="207" spans="2:8" x14ac:dyDescent="0.25">
@@ -50544,7 +50553,7 @@
         <v>1382</v>
       </c>
       <c r="G207" s="33" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
     </row>
     <row r="208" spans="2:8" x14ac:dyDescent="0.25">
@@ -50558,7 +50567,7 @@
         <v>1525</v>
       </c>
       <c r="G208" s="33" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.25">
@@ -50572,10 +50581,10 @@
         <v>2405</v>
       </c>
       <c r="G209" s="33" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="H209" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.25">
@@ -50589,7 +50598,7 @@
         <v>1484</v>
       </c>
       <c r="G210" s="33" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.25">
@@ -50615,7 +50624,7 @@
         <v>1405</v>
       </c>
       <c r="G212" s="33" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.25">
@@ -50641,7 +50650,7 @@
         <v>1441</v>
       </c>
       <c r="G214" s="33" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
     </row>
     <row r="215" spans="2:8" x14ac:dyDescent="0.25">
@@ -50655,7 +50664,7 @@
         <v>1489</v>
       </c>
       <c r="G215" s="33" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="216" spans="2:8" x14ac:dyDescent="0.25">
@@ -50669,7 +50678,7 @@
         <v>2481</v>
       </c>
       <c r="G216" s="33" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
     </row>
     <row r="217" spans="2:8" x14ac:dyDescent="0.25">
@@ -50691,7 +50700,7 @@
         <v>2017</v>
       </c>
       <c r="H218" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.25">
@@ -50715,7 +50724,7 @@
         <v>2484</v>
       </c>
       <c r="G221" s="33" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="222" spans="2:8" x14ac:dyDescent="0.25">
@@ -50729,10 +50738,10 @@
         <v>2485</v>
       </c>
       <c r="G222" s="33" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="H222" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="223" spans="2:8" x14ac:dyDescent="0.25">
@@ -50746,7 +50755,7 @@
         <v>2486</v>
       </c>
       <c r="G223" s="33" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="224" spans="2:8" x14ac:dyDescent="0.25">
@@ -50760,7 +50769,7 @@
         <v>3474</v>
       </c>
       <c r="G224" s="33" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="225" spans="2:7" x14ac:dyDescent="0.25">
@@ -50774,7 +50783,7 @@
         <v>2487</v>
       </c>
       <c r="G225" s="33" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="226" spans="2:7" x14ac:dyDescent="0.25">
@@ -50788,7 +50797,7 @@
         <v>2488</v>
       </c>
       <c r="G226" s="33" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="227" spans="2:7" x14ac:dyDescent="0.25">
@@ -50816,7 +50825,7 @@
         <v>2490</v>
       </c>
       <c r="G228" s="33" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
@@ -50830,7 +50839,7 @@
         <v>2491</v>
       </c>
       <c r="G229" s="33" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="230" spans="2:7" x14ac:dyDescent="0.25">
@@ -50844,7 +50853,7 @@
         <v>2492</v>
       </c>
       <c r="G230" s="33" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="231" spans="2:7" x14ac:dyDescent="0.25">
@@ -50858,7 +50867,7 @@
         <v>2493</v>
       </c>
       <c r="G231" s="33" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="232" spans="2:7" x14ac:dyDescent="0.25">
@@ -50872,7 +50881,7 @@
         <v>2494</v>
       </c>
       <c r="G232" s="33" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="233" spans="2:7" x14ac:dyDescent="0.25">
@@ -50886,7 +50895,7 @@
         <v>2495</v>
       </c>
       <c r="G233" s="33" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="234" spans="2:7" x14ac:dyDescent="0.25">
@@ -50915,7 +50924,7 @@
         <v>2498</v>
       </c>
       <c r="G235" s="33" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="236" spans="2:7" x14ac:dyDescent="0.25">
@@ -50929,7 +50938,7 @@
         <v>2499</v>
       </c>
       <c r="G236" s="33" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="237" spans="2:7" x14ac:dyDescent="0.25">
@@ -50943,7 +50952,7 @@
         <v>2500</v>
       </c>
       <c r="G237" s="33" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="238" spans="2:7" x14ac:dyDescent="0.25">
@@ -50957,7 +50966,7 @@
         <v>2501</v>
       </c>
       <c r="G238" s="33" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="239" spans="2:7" x14ac:dyDescent="0.25">
@@ -50971,7 +50980,7 @@
         <v>2502</v>
       </c>
       <c r="G239" s="33" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="240" spans="2:7" x14ac:dyDescent="0.25">
@@ -50985,7 +50994,7 @@
         <v>2503</v>
       </c>
       <c r="G240" s="33" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="241" spans="2:8" x14ac:dyDescent="0.25">
@@ -51023,7 +51032,7 @@
         <v>2506</v>
       </c>
       <c r="G243" s="33" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="244" spans="2:8" x14ac:dyDescent="0.25">
@@ -51049,7 +51058,7 @@
         <v>2508</v>
       </c>
       <c r="G245" s="33" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
     </row>
     <row r="246" spans="2:8" x14ac:dyDescent="0.25">
@@ -51075,7 +51084,7 @@
         <v>1448</v>
       </c>
       <c r="G247" s="33" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
     </row>
     <row r="248" spans="2:8" x14ac:dyDescent="0.25">
@@ -51089,7 +51098,7 @@
         <v>2509</v>
       </c>
       <c r="G248" s="33" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="249" spans="2:8" x14ac:dyDescent="0.25">
@@ -51103,7 +51112,7 @@
         <v>2510</v>
       </c>
       <c r="G249" s="33" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="250" spans="2:8" x14ac:dyDescent="0.25">
@@ -51117,7 +51126,7 @@
         <v>2511</v>
       </c>
       <c r="G250" s="33" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="251" spans="2:8" x14ac:dyDescent="0.25">
@@ -51131,7 +51140,7 @@
         <v>2512</v>
       </c>
       <c r="G251" s="33" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="252" spans="2:8" x14ac:dyDescent="0.25">
@@ -51145,7 +51154,7 @@
         <v>2513</v>
       </c>
       <c r="G252" s="33" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="253" spans="2:8" x14ac:dyDescent="0.25">
@@ -51159,7 +51168,7 @@
         <v>2514</v>
       </c>
       <c r="G253" s="33" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="254" spans="2:8" x14ac:dyDescent="0.25">
@@ -51173,7 +51182,7 @@
         <v>2515</v>
       </c>
       <c r="G254" s="33" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="255" spans="2:8" x14ac:dyDescent="0.25">
@@ -51187,7 +51196,7 @@
         <v>2516</v>
       </c>
       <c r="G255" s="33" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="256" spans="2:8" x14ac:dyDescent="0.25">
@@ -51201,10 +51210,10 @@
         <v>2517</v>
       </c>
       <c r="G256" s="33" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="H256" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="257" spans="2:8" x14ac:dyDescent="0.25">
@@ -51218,7 +51227,7 @@
         <v>2518</v>
       </c>
       <c r="G257" s="33" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="258" spans="2:8" x14ac:dyDescent="0.25">
@@ -51232,7 +51241,7 @@
         <v>2519</v>
       </c>
       <c r="G258" s="33" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="259" spans="2:8" x14ac:dyDescent="0.25">
@@ -51246,7 +51255,7 @@
         <v>2520</v>
       </c>
       <c r="G259" s="33" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="260" spans="2:8" x14ac:dyDescent="0.25">
@@ -51260,7 +51269,7 @@
         <v>2521</v>
       </c>
       <c r="G260" s="33" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="261" spans="2:8" x14ac:dyDescent="0.25">
@@ -51274,7 +51283,7 @@
         <v>2522</v>
       </c>
       <c r="G261" s="33" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="262" spans="2:8" x14ac:dyDescent="0.25">
@@ -51288,7 +51297,7 @@
         <v>2523</v>
       </c>
       <c r="G262" s="33" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="263" spans="2:8" x14ac:dyDescent="0.25">
@@ -51316,7 +51325,7 @@
         <v>2524</v>
       </c>
       <c r="G264" s="33" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="265" spans="2:8" x14ac:dyDescent="0.25">
@@ -51330,7 +51339,7 @@
         <v>1458</v>
       </c>
       <c r="G265" s="33" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="266" spans="2:8" x14ac:dyDescent="0.25">
@@ -51344,10 +51353,10 @@
         <v>1513</v>
       </c>
       <c r="G266" s="33" t="s">
+        <v>3540</v>
+      </c>
+      <c r="H266" t="s">
         <v>3541</v>
-      </c>
-      <c r="H266" t="s">
-        <v>3542</v>
       </c>
     </row>
     <row r="267" spans="2:8" x14ac:dyDescent="0.25">
@@ -51361,10 +51370,10 @@
         <v>2525</v>
       </c>
       <c r="G267" s="33" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="H267" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="268" spans="2:8" x14ac:dyDescent="0.25">
@@ -51378,7 +51387,7 @@
         <v>2526</v>
       </c>
       <c r="G268" s="33" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="269" spans="2:8" x14ac:dyDescent="0.25">
@@ -51392,7 +51401,7 @@
         <v>2527</v>
       </c>
       <c r="G269" s="33" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="270" spans="2:8" x14ac:dyDescent="0.25">
@@ -51406,7 +51415,7 @@
         <v>2528</v>
       </c>
       <c r="G270" s="33" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="271" spans="2:8" x14ac:dyDescent="0.25">
@@ -51432,7 +51441,7 @@
         <v>1357</v>
       </c>
       <c r="G272" s="33" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="273" spans="2:8" x14ac:dyDescent="0.25">
@@ -51446,7 +51455,7 @@
         <v>1356</v>
       </c>
       <c r="G273" s="33" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="274" spans="2:8" x14ac:dyDescent="0.25">
@@ -51460,7 +51469,7 @@
         <v>1392</v>
       </c>
       <c r="G274" s="33" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="275" spans="2:8" x14ac:dyDescent="0.25">
@@ -51474,7 +51483,7 @@
         <v>1512</v>
       </c>
       <c r="G275" s="33" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="276" spans="2:8" x14ac:dyDescent="0.25">
@@ -51488,7 +51497,7 @@
         <v>1518</v>
       </c>
       <c r="G276" s="33" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="277" spans="2:8" x14ac:dyDescent="0.25">
@@ -51502,7 +51511,7 @@
         <v>1324</v>
       </c>
       <c r="G277" s="33" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="278" spans="2:8" x14ac:dyDescent="0.25">
@@ -51516,7 +51525,7 @@
         <v>1523</v>
       </c>
       <c r="G278" s="33" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="279" spans="2:8" x14ac:dyDescent="0.25">
@@ -51530,7 +51539,7 @@
         <v>1578</v>
       </c>
       <c r="G279" s="33" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
@@ -51544,7 +51553,7 @@
         <v>2530</v>
       </c>
       <c r="G280" s="33" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="281" spans="2:8" x14ac:dyDescent="0.25">
@@ -51572,7 +51581,7 @@
         <v>2531</v>
       </c>
       <c r="G282" s="33" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="283" spans="2:8" x14ac:dyDescent="0.25">
@@ -51586,7 +51595,7 @@
         <v>1495</v>
       </c>
       <c r="G283" s="33" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
     </row>
     <row r="284" spans="2:8" x14ac:dyDescent="0.25">
@@ -51612,7 +51621,7 @@
         <v>1413</v>
       </c>
       <c r="G285" s="33" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
     </row>
     <row r="286" spans="2:8" x14ac:dyDescent="0.25">
@@ -51626,7 +51635,7 @@
         <v>1585</v>
       </c>
       <c r="G286" s="33" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="287" spans="2:8" x14ac:dyDescent="0.25">
@@ -51640,7 +51649,7 @@
         <v>1437</v>
       </c>
       <c r="G287" s="33" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="288" spans="2:8" x14ac:dyDescent="0.25">
@@ -51651,10 +51660,10 @@
         <v>1575</v>
       </c>
       <c r="G288" s="33" t="s">
+        <v>3636</v>
+      </c>
+      <c r="H288" t="s">
         <v>3637</v>
-      </c>
-      <c r="H288" t="s">
-        <v>3638</v>
       </c>
     </row>
     <row r="289" spans="3:8" x14ac:dyDescent="0.25">
@@ -51665,10 +51674,10 @@
         <v>1320</v>
       </c>
       <c r="G289" s="33" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="H289" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="290" spans="3:8" x14ac:dyDescent="0.25">
@@ -51682,7 +51691,7 @@
         <v>3471</v>
       </c>
       <c r="H290" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="291" spans="3:8" x14ac:dyDescent="0.25">
@@ -51693,10 +51702,10 @@
         <v>1423</v>
       </c>
       <c r="G291" s="33" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="H291" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="292" spans="3:8" x14ac:dyDescent="0.25">
@@ -51708,10 +51717,10 @@
         <v>1419</v>
       </c>
       <c r="G292" s="33" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="H292" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="293" spans="3:8" x14ac:dyDescent="0.25">
@@ -51722,10 +51731,10 @@
         <v>1385</v>
       </c>
       <c r="G293" s="33" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="H293" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="294" spans="3:8" x14ac:dyDescent="0.25">
@@ -51736,10 +51745,10 @@
         <v>1451</v>
       </c>
       <c r="G294" s="33" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="H294" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="295" spans="3:8" x14ac:dyDescent="0.25">
@@ -51750,10 +51759,10 @@
         <v>1373</v>
       </c>
       <c r="G295" s="33" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="H295" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="296" spans="3:8" x14ac:dyDescent="0.25">
@@ -51764,10 +51773,10 @@
         <v>1440</v>
       </c>
       <c r="G296" s="33" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="H296" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="297" spans="3:8" x14ac:dyDescent="0.25">
@@ -51778,10 +51787,10 @@
         <v>1482</v>
       </c>
       <c r="G297" s="33" t="s">
+        <v>3644</v>
+      </c>
+      <c r="H297" t="s">
         <v>3645</v>
-      </c>
-      <c r="H297" t="s">
-        <v>3646</v>
       </c>
     </row>
     <row r="298" spans="3:8" x14ac:dyDescent="0.25">
@@ -51792,7 +51801,7 @@
         <v>1566</v>
       </c>
       <c r="G298" s="33" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="299" spans="3:8" x14ac:dyDescent="0.25">
@@ -51803,10 +51812,10 @@
         <v>1310</v>
       </c>
       <c r="G299" s="33" t="s">
+        <v>3647</v>
+      </c>
+      <c r="H299" t="s">
         <v>3648</v>
-      </c>
-      <c r="H299" t="s">
-        <v>3649</v>
       </c>
     </row>
     <row r="300" spans="3:8" x14ac:dyDescent="0.25">
@@ -51817,7 +51826,7 @@
         <v>1407</v>
       </c>
       <c r="G300" s="33" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="301" spans="3:8" x14ac:dyDescent="0.25">
@@ -51828,7 +51837,7 @@
         <v>1339</v>
       </c>
       <c r="G301" s="33" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="302" spans="3:8" x14ac:dyDescent="0.25">
@@ -51839,7 +51848,7 @@
         <v>1411</v>
       </c>
       <c r="G302" s="33" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="303" spans="3:8" x14ac:dyDescent="0.25">
@@ -51850,7 +51859,7 @@
         <v>1559</v>
       </c>
       <c r="G303" s="33" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="304" spans="3:8" x14ac:dyDescent="0.25">
@@ -51861,7 +51870,7 @@
         <v>1312</v>
       </c>
       <c r="G304" s="33" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -51872,7 +51881,7 @@
         <v>2532</v>
       </c>
       <c r="G305" s="33" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
@@ -51883,10 +51892,10 @@
         <v>1418</v>
       </c>
       <c r="G306" s="33" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="H306" s="44" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
@@ -51897,7 +51906,7 @@
         <v>1801</v>
       </c>
       <c r="G307" s="33" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
@@ -51908,7 +51917,7 @@
         <v>1334</v>
       </c>
       <c r="G308" s="33" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
@@ -51919,10 +51928,10 @@
         <v>1521</v>
       </c>
       <c r="G309" s="33" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="H309" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
@@ -51942,10 +51951,10 @@
         <v>1526</v>
       </c>
       <c r="G311" s="33" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="H311" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -51956,10 +51965,10 @@
         <v>1584</v>
       </c>
       <c r="G312" s="33" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="H312" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.25">
@@ -51970,10 +51979,10 @@
         <v>2727</v>
       </c>
       <c r="G313" s="33" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="H313" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -51984,7 +51993,7 @@
         <v>2729</v>
       </c>
       <c r="G314" s="33" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.25">
@@ -51995,7 +52004,7 @@
         <v>1379</v>
       </c>
       <c r="G315" s="33" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.25">
@@ -52015,7 +52024,7 @@
         <v>1569</v>
       </c>
       <c r="G316" s="33" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.25">
@@ -52055,7 +52064,7 @@
         <v>1465</v>
       </c>
       <c r="G318" s="33" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.25">
@@ -52075,7 +52084,7 @@
         <v>1499</v>
       </c>
       <c r="G319" s="33" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.25">
@@ -52133,7 +52142,7 @@
         <v>1486</v>
       </c>
       <c r="G322" s="33" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.25">
@@ -52153,7 +52162,7 @@
         <v>1496</v>
       </c>
       <c r="G323" s="33" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.25">
@@ -52173,7 +52182,7 @@
         <v>1562</v>
       </c>
       <c r="G324" s="33" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.25">
@@ -52211,7 +52220,7 @@
         <v>1537</v>
       </c>
       <c r="G326" s="33" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.25">
@@ -52231,7 +52240,7 @@
         <v>1488</v>
       </c>
       <c r="G327" s="33" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
     </row>
     <row r="328" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -52251,7 +52260,7 @@
         <v>1434</v>
       </c>
       <c r="G328" s="33" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.25">
@@ -52262,7 +52271,7 @@
         <v>1375</v>
       </c>
       <c r="G329" s="33" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.25">
@@ -52276,10 +52285,10 @@
         <v>1456</v>
       </c>
       <c r="G330" s="33" t="s">
+        <v>3671</v>
+      </c>
+      <c r="H330" t="s">
         <v>3672</v>
-      </c>
-      <c r="H330" t="s">
-        <v>3673</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.25">
@@ -52290,7 +52299,7 @@
         <v>1553</v>
       </c>
       <c r="G331" s="33" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.25">
@@ -52301,7 +52310,7 @@
         <v>2760</v>
       </c>
       <c r="G332" s="33" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.25">
@@ -52312,7 +52321,7 @@
         <v>2762</v>
       </c>
       <c r="G333" s="33" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.25">
@@ -52323,7 +52332,7 @@
         <v>1581</v>
       </c>
       <c r="G334" s="33" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.25">
@@ -52334,7 +52343,7 @@
         <v>2765</v>
       </c>
       <c r="G335" s="33" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.25">
@@ -52362,7 +52371,7 @@
         <v>3176</v>
       </c>
       <c r="H337" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="338" spans="2:8" x14ac:dyDescent="0.25">
@@ -52605,8 +52614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED3E70-2200-4646-9295-321DD5DC5132}">
   <dimension ref="B6:AF108"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54295,11 +54304,11 @@
     </row>
     <row r="108" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H108" s="35" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
       <c r="I108" s="35"/>
       <c r="J108" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>